<commit_message>
integrating book_recomendation and main intent classification
</commit_message>
<xml_diff>
--- a/train.xlsx
+++ b/train.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rusdi-prototype-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rusdi-prototype-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8C5B20-71ED-4663-92AA-5461D53299ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA649256-F263-4A65-9341-C6E4BD6326C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="718">
   <si>
     <t>text</t>
   </si>
@@ -3028,8 +3028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A707" workbookViewId="0">
-      <selection activeCell="A724" sqref="A724"/>
+    <sheetView tabSelected="1" topLeftCell="A709" workbookViewId="0">
+      <selection activeCell="B713" sqref="B713:B721"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8633,115 +8633,184 @@
       <c r="A699" t="s">
         <v>695</v>
       </c>
+      <c r="B699" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
         <v>696</v>
       </c>
+      <c r="B700" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
         <v>697</v>
       </c>
+      <c r="B701" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
         <v>698</v>
       </c>
+      <c r="B702" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
         <v>699</v>
       </c>
+      <c r="B703" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="705" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B704" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="706" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B705" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="707" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B706" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="708" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B707" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="709" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B708" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="710" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B709" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="711" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B710" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="712" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B711" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="713" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B712" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="714" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B713" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="715" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B714" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="716" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B715" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="717" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B716" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="718" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B717" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="719" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B718" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="720" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B719" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="721" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B720" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
         <v>717</v>
+      </c>
+      <c r="B721" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>